<commit_message>
updating input file names, making forecast structure configurable, adding index sheet to input excel
</commit_message>
<xml_diff>
--- a/src_files/unitdata_additional-conventional-units.xlsx
+++ b/src_files/unitdata_additional-conventional-units.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8E11BE-45A1-4D13-BBF2-48D61205620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B958F73A-4056-461D-AC2F-1846CBA39B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitdata" sheetId="1" r:id="rId1"/>
     <sheet name="Remove_units_by_node" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">unitdata!$A$1:$F$167</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">unitdata!$A$1:$F$175</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="50">
   <si>
     <t>Node</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Battery discharger</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -517,7 +520,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -551,7 +554,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -585,7 +588,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -619,7 +622,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -636,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -670,7 +673,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -704,7 +707,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -721,7 +724,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -874,7 +877,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -891,7 +894,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -925,7 +928,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -1263,7 +1266,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -1314,7 +1317,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>14</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>22</v>
       </c>
@@ -1501,7 +1504,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>22</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>16</v>
       </c>
@@ -1603,7 +1606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>16</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>17</v>
       </c>
@@ -1654,7 +1657,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>17</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>33</v>
       </c>
@@ -1739,7 +1742,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>35</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>35</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>34</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>34</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>9</v>
       </c>
@@ -2096,7 +2099,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>12</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>13</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>14</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>14</v>
       </c>
@@ -2215,7 +2218,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>16</v>
       </c>
@@ -2249,7 +2252,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>17</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>4875</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>22</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>22</v>
       </c>
@@ -2334,7 +2337,7 @@
         <v>2275</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>26</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>26</v>
       </c>
@@ -2963,7 +2966,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>38</v>
       </c>
@@ -3048,7 +3051,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>38</v>
       </c>
@@ -3082,7 +3085,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>21</v>
       </c>
@@ -3099,7 +3102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>21</v>
       </c>
@@ -3184,7 +3187,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>9</v>
       </c>
@@ -3201,7 +3204,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>12</v>
       </c>
@@ -3235,7 +3238,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>26</v>
       </c>
@@ -3252,7 +3255,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>27</v>
       </c>
@@ -3269,7 +3272,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>35</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>22</v>
       </c>
@@ -3303,7 +3306,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>34</v>
       </c>
@@ -3320,12 +3323,148 @@
         <v>5000</v>
       </c>
     </row>
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>9</v>
+      </c>
+      <c r="B168" t="s">
+        <v>49</v>
+      </c>
+      <c r="C168" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168">
+        <v>2025</v>
+      </c>
+      <c r="E168">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>22</v>
+      </c>
+      <c r="B169" t="s">
+        <v>49</v>
+      </c>
+      <c r="C169" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169">
+        <v>2025</v>
+      </c>
+      <c r="E169">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>25</v>
+      </c>
+      <c r="B170" t="s">
+        <v>49</v>
+      </c>
+      <c r="C170" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170">
+        <v>2025</v>
+      </c>
+      <c r="E170">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>26</v>
+      </c>
+      <c r="B171" t="s">
+        <v>49</v>
+      </c>
+      <c r="C171" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171">
+        <v>2025</v>
+      </c>
+      <c r="E171">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>27</v>
+      </c>
+      <c r="B172" t="s">
+        <v>49</v>
+      </c>
+      <c r="C172" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172">
+        <v>2025</v>
+      </c>
+      <c r="E172">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>35</v>
+      </c>
+      <c r="B173" t="s">
+        <v>49</v>
+      </c>
+      <c r="C173" t="s">
+        <v>29</v>
+      </c>
+      <c r="D173">
+        <v>2040</v>
+      </c>
+      <c r="E173">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>22</v>
+      </c>
+      <c r="B174" t="s">
+        <v>49</v>
+      </c>
+      <c r="C174" t="s">
+        <v>29</v>
+      </c>
+      <c r="D174">
+        <v>2040</v>
+      </c>
+      <c r="E174">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>34</v>
+      </c>
+      <c r="B175" t="s">
+        <v>49</v>
+      </c>
+      <c r="C175" t="s">
+        <v>29</v>
+      </c>
+      <c r="D175">
+        <v>2040</v>
+      </c>
+      <c r="E175">
+        <v>5000</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F167" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:F175" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Battery charger"/>
-        <filter val="Battery discharger"/>
+        <filter val="Hydrogen processor"/>
+        <filter val="Hydrogen storage dimensioner"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>